<commit_message>
Continuing WIP, databook read and write seems functional
</commit_message>
<xml_diff>
--- a/atomica/library/environment_framework.xlsx
+++ b/atomica/library/environment_framework.xlsx
@@ -1,32 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF54AE8-DB85-4DCC-A84B-35F6D13DFF02}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14869335-F5ED-466E-94BB-4D0232AF2757}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="2400" windowWidth="28065" windowHeight="17190" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7740" yWindow="2400" windowWidth="28065" windowHeight="17190" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Databook Pages" sheetId="2" r:id="rId2"/>
     <sheet name="Compartments" sheetId="3" r:id="rId3"/>
-    <sheet name="Transitions" sheetId="4" r:id="rId4"/>
-    <sheet name="Characteristics" sheetId="5" r:id="rId5"/>
-    <sheet name="Parameters" sheetId="6" r:id="rId6"/>
-    <sheet name="Cascades" sheetId="7" r:id="rId7"/>
+    <sheet name="Population types" sheetId="8" r:id="rId4"/>
+    <sheet name="Transitions" sheetId="4" r:id="rId5"/>
+    <sheet name="Characteristics" sheetId="5" r:id="rId6"/>
+    <sheet name="Parameters" sheetId="6" r:id="rId7"/>
+    <sheet name="Cascades" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -280,6 +280,82 @@
     <author>None</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{9CED2BE4-0376-44EB-8541-F112D3A63E72}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>This column is for the 'code name' of a custom databook sheet.
+Normally, when constructing a databook, data-input sections for
+compartments and characteristics are placed on a single page, while
+parameters are placed on another.
+This section allows custom sheets to be defined, allowing for more
+user-friendly databook organisation.
+Note: A code name is a representative key that developers interface
+with (e.g. in scripts and the codebase).
+It should be in lower case without spaces.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{61C08625-CB24-4773-AD83-3651FEC7EE18}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>This column is for the title of a custom databook sheet.
+Normally, when constructing a databook, data-input sections for
+compartments and characteristics are placed on a single page, while
+parameters are placed on another.
+This section allows custom sheets to be defined, allowing for more
+user-friendly databook organisation.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Romesh</author>
+  </authors>
+  <commentList>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{6CDFEB27-B50E-411A-B710-D2268E8C4E81}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Romesh:
+The transition matrix specifies which transitions exist and which parameter governs them. Transitions go from row to column</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>None</author>
+  </authors>
+  <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
@@ -437,7 +513,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>None</author>
@@ -504,7 +580,35 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{E3F9A7D1-69EC-4661-81E3-DA6D1FC4EA95}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>If you specify a minimum value, the parameter will never drop below this value. If included, it would typically be 0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{7DFA201F-E0DD-437A-BCE1-9EEA727BD836}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>If you specify a maximum value, the parameter will never exceed this value. A common use would be to ensure that a probability cannot be larger than 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
         <r>
           <rPr>
@@ -518,7 +622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000005000000}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000005000000}">
       <text>
         <r>
           <rPr>
@@ -532,7 +636,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000006000000}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000006000000}">
       <text>
         <r>
           <rPr>
@@ -551,7 +655,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -772,12 +876,6 @@
     <t>inf,rec</t>
   </si>
   <si>
-    <t>Environment</t>
-  </si>
-  <si>
-    <t>environment</t>
-  </si>
-  <si>
     <t>Population type</t>
   </si>
   <si>
@@ -788,6 +886,123 @@
   </si>
   <si>
     <t>SRC_POP_SUM(foi)</t>
+  </si>
+  <si>
+    <t>undx</t>
+  </si>
+  <si>
+    <t>Undiagnosed</t>
+  </si>
+  <si>
+    <t>dx</t>
+  </si>
+  <si>
+    <t>Diagnosed</t>
+  </si>
+  <si>
+    <t>tx</t>
+  </si>
+  <si>
+    <t>Treated</t>
+  </si>
+  <si>
+    <t>Code name</t>
+  </si>
+  <si>
+    <t>sir</t>
+  </si>
+  <si>
+    <t>udt</t>
+  </si>
+  <si>
+    <t>UDT</t>
+  </si>
+  <si>
+    <t>diag</t>
+  </si>
+  <si>
+    <t>initiate</t>
+  </si>
+  <si>
+    <t>loss</t>
+  </si>
+  <si>
+    <t>all_people</t>
+  </si>
+  <si>
+    <t>All people with condition</t>
+  </si>
+  <si>
+    <t>undx, dx, tx</t>
+  </si>
+  <si>
+    <t>stocks</t>
+  </si>
+  <si>
+    <t>all_dx</t>
+  </si>
+  <si>
+    <t>Diagnosed people</t>
+  </si>
+  <si>
+    <t>dx, tx</t>
+  </si>
+  <si>
+    <t>all_tx</t>
+  </si>
+  <si>
+    <t>Currently treated</t>
+  </si>
+  <si>
+    <t>num_diag</t>
+  </si>
+  <si>
+    <t>Annual number of new diagnoses</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>flows</t>
+  </si>
+  <si>
+    <t>Diagnosis rate</t>
+  </si>
+  <si>
+    <t>probability</t>
+  </si>
+  <si>
+    <t>num_diag/max(undx,num_diag)</t>
+  </si>
+  <si>
+    <t>num_initiate</t>
+  </si>
+  <si>
+    <t>Annual number newly initiated onto treatment</t>
+  </si>
+  <si>
+    <t>Initiation rate</t>
+  </si>
+  <si>
+    <t>num_initiate/max(dx,num_initiate)</t>
+  </si>
+  <si>
+    <t>num_loss</t>
+  </si>
+  <si>
+    <t>Annual number lost to follow-up</t>
+  </si>
+  <si>
+    <t>Loss-to-follow-up rate</t>
+  </si>
+  <si>
+    <t>num_loss/max(tx,num_loss)</t>
+  </si>
+  <si>
+    <t>Minimum value</t>
+  </si>
+  <si>
+    <t>Maximum value</t>
   </si>
 </sst>
 </file>
@@ -837,7 +1052,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -855,11 +1070,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1227,7 +1481,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,16 +1553,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="8" width="15.7109375" customWidth="1"/>
+    <col min="2" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1337,7 +1593,7 @@
         <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1361,6 +1617,9 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
+      <c r="I2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1381,6 +1640,9 @@
       <c r="F3" s="3"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
+      <c r="I3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1401,6 +1663,9 @@
       <c r="F4" s="3"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
+      <c r="I4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1421,8 +1686,53 @@
       <c r="F5" s="3"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
+      <c r="I5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B7:B9">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>AND(A7&lt;&gt;"",NOT(B7&lt;&gt;""))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:E5" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"n,y"</formula1>
@@ -1434,11 +1744,55 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1DFFE9-89FE-4855-871D-DB0CA70E68DF}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,6 +1805,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
       <c r="B1" s="1" t="str">
         <f>Compartments!A2</f>
         <v>sus</v>
@@ -1507,17 +1864,56 @@
         <v>dead</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,10 +1925,10 @@
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1560,11 +1956,8 @@
       <c r="I1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -1581,11 +1974,8 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -1604,9 +1994,8 @@
         <v>35</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -1621,9 +2010,8 @@
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
@@ -1638,9 +2026,8 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
@@ -1655,9 +2042,8 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>49</v>
       </c>
@@ -1674,9 +2060,8 @@
         <v>35</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>51</v>
       </c>
@@ -1693,9 +2078,8 @@
         <v>35</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
@@ -1712,17 +2096,78 @@
         <v>35</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="F11" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="I12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B11:B13">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>AND(A11&lt;&gt;"",NOT(B11&lt;&gt;""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:C13">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>AND(#REF!&lt;&gt;"",NOT(C11&lt;&gt;""))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
@@ -1734,14 +2179,14 @@
     <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="107.42578125" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="5" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.7109375" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1755,22 +2200,28 @@
         <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
@@ -1783,16 +2234,21 @@
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="4">
+      <c r="H2" s="2"/>
+      <c r="I2" s="4">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="5"/>
+      <c r="K2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>61</v>
       </c>
@@ -1802,16 +2258,21 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3">
+      <c r="H3" s="2"/>
+      <c r="I3">
         <v>80</v>
       </c>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="5"/>
+      <c r="K3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -1824,16 +2285,21 @@
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4">
+      <c r="H4" s="2"/>
+      <c r="I4">
         <v>0.5</v>
       </c>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="5"/>
+      <c r="K4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>65</v>
       </c>
@@ -1846,16 +2312,21 @@
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="6">
+      <c r="H5" s="2"/>
+      <c r="I5" s="6">
         <v>1.6E-2</v>
       </c>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="5"/>
+      <c r="K5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -1868,16 +2339,21 @@
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="6">
+      <c r="H6" s="2"/>
+      <c r="I6" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="5"/>
+      <c r="K6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
@@ -1890,34 +2366,212 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="H7" s="5" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="J7" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="K7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" t="s">
-        <v>74</v>
+      <c r="K9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="K13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K15" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B10:B15">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>AND(A10&lt;&gt;"",NOT(B10&lt;&gt;""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D14">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>AND(#REF!&lt;&gt;"",NOT(D10&lt;&gt;""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G10:G15" xr:uid="{BCC32A75-D6CD-4587-8FD1-383D483B76E5}">
+      <formula1>"y,n"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C10:C15" xr:uid="{62C14FD9-43E3-4853-8F16-2A7006D41A94}">
+      <formula1>",number,probability,duration,proportion"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>